<commit_message>
Fixed Errors and Added Missing Scores
Fixed Florida Score on 6/26 and Added missing PA scores
</commit_message>
<xml_diff>
--- a/coviddiary_rawsourcedata_public_08052020/COVID_ALL_G1_data_09302020_public.xlsx
+++ b/coviddiary_rawsourcedata_public_08052020/COVID_ALL_G1_data_09302020_public.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annikaavery/Documents/LakdawalaLab/COVID_Diary/coviddiary_sourcedata/coviddiary_rawsourcedata_public_08052020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CE4544-3169-5F49-8342-DDDB1ED3446E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523144DE-F6E5-D34D-AD78-D75B75C15941}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29240" yWindow="-13260" windowWidth="17080" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4360" yWindow="460" windowWidth="19500" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -998,7 +998,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1025,6 +1025,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1331,8 +1332,8 @@
   <dimension ref="A1:N690"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I135" sqref="I135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7268,7 +7269,7 @@
         <v>36</v>
       </c>
       <c r="I135" s="6">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="J135">
         <v>294478</v>
@@ -23896,7 +23897,9 @@
       <c r="H513" t="s">
         <v>17</v>
       </c>
-      <c r="I513" s="6"/>
+      <c r="I513" s="6">
+        <v>1</v>
+      </c>
       <c r="J513">
         <v>1779798</v>
       </c>
@@ -23938,7 +23941,9 @@
       <c r="H514" t="s">
         <v>19</v>
       </c>
-      <c r="I514" s="6"/>
+      <c r="I514" s="6">
+        <v>1.75</v>
+      </c>
       <c r="J514">
         <v>1779798</v>
       </c>
@@ -23980,7 +23985,9 @@
       <c r="H515" t="s">
         <v>21</v>
       </c>
-      <c r="I515" s="6"/>
+      <c r="I515" s="6">
+        <v>2.75</v>
+      </c>
       <c r="J515">
         <v>1779798</v>
       </c>
@@ -24022,7 +24029,9 @@
       <c r="H516" t="s">
         <v>23</v>
       </c>
-      <c r="I516" s="6"/>
+      <c r="I516" s="6">
+        <v>3.75</v>
+      </c>
       <c r="J516">
         <v>1779798</v>
       </c>
@@ -24064,7 +24073,9 @@
       <c r="H517" t="s">
         <v>27</v>
       </c>
-      <c r="I517" s="6"/>
+      <c r="I517" s="6">
+        <v>3.65</v>
+      </c>
       <c r="J517">
         <v>1779798</v>
       </c>
@@ -24106,7 +24117,9 @@
       <c r="H518" t="s">
         <v>27</v>
       </c>
-      <c r="I518" s="6"/>
+      <c r="I518" s="6">
+        <v>3.6</v>
+      </c>
       <c r="J518">
         <v>1779798</v>
       </c>
@@ -24148,7 +24161,9 @@
       <c r="H519" t="s">
         <v>27</v>
       </c>
-      <c r="I519" s="6"/>
+      <c r="I519" s="6">
+        <v>3.55</v>
+      </c>
       <c r="J519">
         <v>1779798</v>
       </c>
@@ -24190,7 +24205,9 @@
       <c r="H520" t="s">
         <v>27</v>
       </c>
-      <c r="I520" s="6"/>
+      <c r="I520" s="6">
+        <v>3.25</v>
+      </c>
       <c r="J520">
         <v>1779798</v>
       </c>
@@ -24232,7 +24249,9 @@
       <c r="H521" t="s">
         <v>25</v>
       </c>
-      <c r="I521" s="6"/>
+      <c r="I521" s="6">
+        <v>2.25</v>
+      </c>
       <c r="J521">
         <v>1779798</v>
       </c>
@@ -24274,7 +24293,9 @@
       <c r="H522" t="s">
         <v>27</v>
       </c>
-      <c r="I522" s="6"/>
+      <c r="I522" s="6">
+        <v>1.55</v>
+      </c>
       <c r="J522">
         <v>1779798</v>
       </c>
@@ -24316,7 +24337,9 @@
       <c r="H523" t="s">
         <v>85</v>
       </c>
-      <c r="I523" s="6"/>
+      <c r="I523" s="6">
+        <v>1.55</v>
+      </c>
       <c r="J523">
         <v>1779798</v>
       </c>
@@ -24358,7 +24381,9 @@
       <c r="H524" t="s">
         <v>31</v>
       </c>
-      <c r="I524" s="6"/>
+      <c r="I524" s="6">
+        <v>1.55</v>
+      </c>
       <c r="J524">
         <v>1779798</v>
       </c>
@@ -24400,7 +24425,9 @@
       <c r="H525" t="s">
         <v>34</v>
       </c>
-      <c r="I525" s="6"/>
+      <c r="I525" s="6">
+        <v>2.5499999999999998</v>
+      </c>
       <c r="J525">
         <v>1779798</v>
       </c>
@@ -24442,7 +24469,9 @@
       <c r="H526" t="s">
         <v>52</v>
       </c>
-      <c r="I526" s="6"/>
+      <c r="I526" s="6">
+        <v>3.45</v>
+      </c>
       <c r="J526">
         <v>1779798</v>
       </c>
@@ -24484,7 +24513,9 @@
       <c r="H527" t="s">
         <v>142</v>
       </c>
-      <c r="I527" s="6"/>
+      <c r="I527" s="6">
+        <v>3.45</v>
+      </c>
       <c r="J527">
         <v>1779798</v>
       </c>
@@ -24526,7 +24557,9 @@
       <c r="H528" t="s">
         <v>36</v>
       </c>
-      <c r="I528" s="6"/>
+      <c r="I528" s="6">
+        <v>3.45</v>
+      </c>
       <c r="J528">
         <v>1779798</v>
       </c>
@@ -24543,7 +24576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="529" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="529" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A529" t="s">
         <v>211</v>
       </c>
@@ -24568,8 +24601,8 @@
       <c r="H529" t="s">
         <v>19</v>
       </c>
-      <c r="I529" s="7">
-        <v>2</v>
+      <c r="I529" s="14">
+        <v>3.45</v>
       </c>
       <c r="J529">
         <v>1219835</v>

</xml_diff>